<commit_message>
Updated Code Review file
</commit_message>
<xml_diff>
--- a/Code Review.xlsx
+++ b/Code Review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joego\Documents\sem_cw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eilid\IdeaProjects\sem_cw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5181C776-61A9-4123-BBA5-30F927BD8C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572E6424-7E8E-4658-B724-8557EF1677A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7910A481-4624-436B-8167-C81A2DF3F8BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7910A481-4624-436B-8167-C81A2DF3F8BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Code Review 2</t>
+  </si>
+  <si>
+    <t>Code Review 3</t>
   </si>
 </sst>
 </file>
@@ -409,19 +412,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D98B4D-93BC-4721-8C86-038D64A7F27A}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
     <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,8 +436,11 @@
       <c r="C1" t="s">
         <v>7</v>
       </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -442,8 +450,11 @@
       <c r="C2">
         <v>25</v>
       </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -453,8 +464,11 @@
       <c r="C3">
         <v>25</v>
       </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -464,8 +478,11 @@
       <c r="C4">
         <v>25</v>
       </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -475,8 +492,11 @@
       <c r="C5">
         <v>25</v>
       </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -484,6 +504,9 @@
         <v>100</v>
       </c>
       <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
         <v>100</v>
       </c>
     </row>

</xml_diff>